<commit_message>
updated figure and data
</commit_message>
<xml_diff>
--- a/4_aviation/gdp_rmp_correlation_historical/data/world/data.xlsx
+++ b/4_aviation/gdp_rmp_correlation_historical/data/world/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelweinold/github/phd_publication_figures/4_aviation/gdp_rmp_correlation_historical/data/world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36769B32-97DB-9E4A-BB64-C6BB0619C56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2514FE-41EC-C64F-94C1-AB45FB75D583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{DDCBDB21-DEB9-2846-B64A-BF2BE696C8CF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="27">
   <si>
     <t>..</t>
   </si>
@@ -105,10 +105,19 @@
     <t>world air passenger traffic (Gkm)</t>
   </si>
   <si>
-    <t>world air passenger traffic (km)</t>
+    <t>world air passenger traffic (# people)</t>
   </si>
   <si>
-    <t>plot world air passenger traffic (km)</t>
+    <t>plot world air passenger traffic (# people)</t>
+  </si>
+  <si>
+    <t>world rpk (km)</t>
+  </si>
+  <si>
+    <t>https://ourworldindata.org/grapher/airline-capacity-and-traffic</t>
+  </si>
+  <si>
+    <t>plot world rpk (km)</t>
   </si>
 </sst>
 </file>
@@ -480,7 +489,7 @@
   <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4742,20 +4751,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5528D731-BC45-EA41-A6A0-5D051D7EC5E6}">
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="O74" sqref="O74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4793,13 +4803,22 @@
         <v>4</v>
       </c>
       <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1950</v>
       </c>
@@ -4840,15 +4859,25 @@
         <v>13</v>
       </c>
       <c r="M2">
+        <v>28000000000</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2">
         <f>D2</f>
         <v>880959417787.24268</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <f>I2</f>
         <v>17879948.914431199</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q2">
+        <f>M2</f>
+        <v>28000000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1951</v>
       </c>
@@ -4889,15 +4918,25 @@
         <v>13</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M12" si="3">D3</f>
+        <v>35000000000</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O12" si="3">D3</f>
         <v>932817426817.64697</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N24" si="4">I3</f>
+      <c r="P3">
+        <f t="shared" ref="P3:P24" si="4">I3</f>
         <v>31289910.600255299</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q66" si="5">M3</f>
+        <v>35000000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1952</v>
       </c>
@@ -4938,15 +4977,25 @@
         <v>13</v>
       </c>
       <c r="M4">
+        <v>40000000000</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4">
         <f t="shared" si="3"/>
         <v>975961815802.85645</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <f t="shared" si="4"/>
         <v>35759897.828862898</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q4">
+        <f t="shared" si="5"/>
+        <v>40000000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1953</v>
       </c>
@@ -4987,15 +5036,25 @@
         <v>13</v>
       </c>
       <c r="M5">
+        <v>47000000000</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5">
         <f t="shared" si="3"/>
         <v>1025114207006.4968</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <f t="shared" si="4"/>
         <v>44699872.2860789</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q5">
+        <f t="shared" si="5"/>
+        <v>47000000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1954</v>
       </c>
@@ -5036,15 +5095,25 @@
         <v>13</v>
       </c>
       <c r="M6">
+        <v>52000000000</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6">
         <f t="shared" si="3"/>
         <v>1060154826981.7273</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <f t="shared" si="4"/>
         <v>49169859.514686994</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q6">
+        <f t="shared" si="5"/>
+        <v>52000000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1955</v>
       </c>
@@ -5085,15 +5154,25 @@
         <v>13</v>
       </c>
       <c r="M7">
+        <v>61000000000</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7">
         <f t="shared" si="3"/>
         <v>1127730466073.0176</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <f t="shared" si="4"/>
         <v>58109833.971903004</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q7">
+        <f t="shared" si="5"/>
+        <v>61000000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1956</v>
       </c>
@@ -5134,15 +5213,25 @@
         <v>13</v>
       </c>
       <c r="M8">
+        <v>71000000000</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8">
         <f t="shared" si="3"/>
         <v>1180760859037.625</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <f t="shared" si="4"/>
         <v>67049808.429118201</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q8">
+        <f t="shared" si="5"/>
+        <v>71000000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1957</v>
       </c>
@@ -5183,15 +5272,25 @@
         <v>13</v>
       </c>
       <c r="M9">
+        <v>82000000000</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9">
         <f t="shared" si="3"/>
         <v>1225697618734.4587</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <f t="shared" si="4"/>
         <v>75989782.886334211</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q9">
+        <f t="shared" si="5"/>
+        <v>82000000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1958</v>
       </c>
@@ -5232,15 +5331,25 @@
         <v>13</v>
       </c>
       <c r="M10">
+        <v>85000000000</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10">
         <f t="shared" si="3"/>
         <v>1265056296253.155</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <f t="shared" si="4"/>
         <v>80459770.114942312</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q10">
+        <f t="shared" si="5"/>
+        <v>85000000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1959</v>
       </c>
@@ -5281,15 +5390,25 @@
         <v>13</v>
       </c>
       <c r="M11">
+        <v>98000000000</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11">
         <f t="shared" si="3"/>
         <v>1323034035613.6702</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <f t="shared" si="4"/>
         <v>89399744.57215789</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q11">
+        <f t="shared" si="5"/>
+        <v>98000000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1960</v>
       </c>
@@ -5330,15 +5449,25 @@
         <v>13</v>
       </c>
       <c r="M12">
+        <v>109000000000</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12">
         <f t="shared" si="3"/>
         <v>1392273064404.3333</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <f t="shared" si="4"/>
         <v>102809706.257982</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q12">
+        <f t="shared" si="5"/>
+        <v>109000000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1961</v>
       </c>
@@ -5377,15 +5506,25 @@
         <v>13</v>
       </c>
       <c r="M13">
+        <v>117000000000</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13">
         <f>F13</f>
         <v>1448621687210.3347</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <f t="shared" si="4"/>
         <v>98339719.029373989</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q13">
+        <f t="shared" si="5"/>
+        <v>117000000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1962</v>
       </c>
@@ -5424,15 +5563,25 @@
         <v>13</v>
       </c>
       <c r="M14">
-        <f t="shared" ref="M14:M74" si="5">F14</f>
+        <v>130000000000</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ref="O14:O74" si="6">F14</f>
         <v>1550544284536.876</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <f t="shared" si="4"/>
         <v>111749680.715198</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q14">
+        <f t="shared" si="5"/>
+        <v>130000000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1963</v>
       </c>
@@ -5471,15 +5620,25 @@
         <v>13</v>
       </c>
       <c r="M15">
-        <f t="shared" si="5"/>
+        <v>147000000000</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="6"/>
         <v>1671610129796.687</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <f t="shared" si="4"/>
         <v>125159642.401021</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q15">
+        <f t="shared" si="5"/>
+        <v>147000000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1964</v>
       </c>
@@ -5518,15 +5677,25 @@
         <v>13</v>
       </c>
       <c r="M16">
-        <f t="shared" si="5"/>
+        <v>171000000000</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="6"/>
         <v>1830287415820.9106</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <f t="shared" si="4"/>
         <v>143039591.31545198</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q16">
+        <f t="shared" si="5"/>
+        <v>171000000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1965</v>
       </c>
@@ -5565,15 +5734,25 @@
         <v>13</v>
       </c>
       <c r="M17">
-        <f t="shared" si="5"/>
+        <v>198000000000</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="6"/>
         <v>1993900164077.1504</v>
       </c>
-      <c r="N17">
+      <c r="P17">
         <f t="shared" si="4"/>
         <v>165389527.45849299</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q17">
+        <f t="shared" si="5"/>
+        <v>198000000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1966</v>
       </c>
@@ -5612,15 +5791,25 @@
         <v>13</v>
       </c>
       <c r="M18">
-        <f t="shared" si="5"/>
+        <v>229000000000</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="6"/>
         <v>2163893762205.561</v>
       </c>
-      <c r="N18">
+      <c r="P18">
         <f t="shared" si="4"/>
         <v>192209450.83013898</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q18">
+        <f t="shared" si="5"/>
+        <v>229000000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1967</v>
       </c>
@@ -5659,15 +5848,25 @@
         <v>13</v>
       </c>
       <c r="M19">
-        <f t="shared" si="5"/>
+        <v>273000000000</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="6"/>
         <v>2302529133110.2158</v>
       </c>
-      <c r="N19">
+      <c r="P19">
         <f t="shared" si="4"/>
         <v>223499361.43039501</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q19">
+        <f t="shared" si="5"/>
+        <v>273000000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1968</v>
       </c>
@@ -5706,15 +5905,25 @@
         <v>13</v>
       </c>
       <c r="M20">
-        <f t="shared" si="5"/>
+        <v>309422000000</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="6"/>
         <v>2485212751062.4946</v>
       </c>
-      <c r="N20">
+      <c r="P20">
         <f t="shared" si="4"/>
         <v>250319284.80204302</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q20">
+        <f t="shared" si="5"/>
+        <v>309422000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1969</v>
       </c>
@@ -5753,15 +5962,25 @@
         <v>13</v>
       </c>
       <c r="M21">
-        <f t="shared" si="5"/>
+        <v>350899000000</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="6"/>
         <v>2741171923549.1372</v>
       </c>
-      <c r="N21">
+      <c r="P21">
         <f t="shared" si="4"/>
         <v>286079182.63090599</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q21">
+        <f t="shared" si="5"/>
+        <v>350899000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1970</v>
       </c>
@@ -5800,15 +6019,25 @@
         <v>19</v>
       </c>
       <c r="M22">
-        <f t="shared" si="5"/>
+        <v>460481000000</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="6"/>
         <v>2997220356779.1016</v>
       </c>
-      <c r="N22">
+      <c r="P22">
         <f t="shared" si="4"/>
         <v>371008939.97445703</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q22">
+        <f t="shared" si="5"/>
+        <v>460481000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1971</v>
       </c>
@@ -5847,15 +6076,25 @@
         <v>19</v>
       </c>
       <c r="M23">
-        <f t="shared" si="5"/>
+        <v>494137000000</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="6"/>
         <v>3310772104445.6387</v>
       </c>
-      <c r="N23">
+      <c r="P23">
         <f t="shared" si="4"/>
         <v>402298850.57471198</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q23">
+        <f t="shared" si="5"/>
+        <v>494137000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1972</v>
       </c>
@@ -5894,15 +6133,25 @@
         <v>19</v>
       </c>
       <c r="M24">
-        <f t="shared" si="5"/>
+        <v>560078000000</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="6"/>
         <v>3817137302147.7573</v>
       </c>
-      <c r="N24">
+      <c r="P24">
         <f t="shared" si="4"/>
         <v>438058748.403575</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q24">
+        <f t="shared" si="5"/>
+        <v>560078000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1973</v>
       </c>
@@ -5940,15 +6189,25 @@
         <v>19</v>
       </c>
       <c r="M25">
-        <f t="shared" si="5"/>
+        <v>618184000000</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="6"/>
         <v>4656966197587.3018</v>
       </c>
-      <c r="N25">
+      <c r="P25">
         <f>K25</f>
         <v>401571800</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q25">
+        <f t="shared" si="5"/>
+        <v>618184000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1974</v>
       </c>
@@ -5986,15 +6245,25 @@
         <v>19</v>
       </c>
       <c r="M26">
+        <v>656426000000</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="6"/>
+        <v>5367575035061.4551</v>
+      </c>
+      <c r="P26">
+        <f>K26</f>
+        <v>421145200</v>
+      </c>
+      <c r="Q26">
         <f t="shared" si="5"/>
-        <v>5367575035061.4551</v>
-      </c>
-      <c r="N26">
-        <f t="shared" ref="N26:N74" si="6">K26</f>
-        <v>421145200</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+        <v>656426000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1975</v>
       </c>
@@ -6032,15 +6301,25 @@
         <v>19</v>
       </c>
       <c r="M27">
+        <v>697285000000</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="6"/>
+        <v>5978906146254.5859</v>
+      </c>
+      <c r="P27">
+        <f>K27</f>
+        <v>432276500</v>
+      </c>
+      <c r="Q27">
         <f t="shared" si="5"/>
-        <v>5978906146254.5859</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="6"/>
-        <v>432276500</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+        <v>697285000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1976</v>
       </c>
@@ -6078,15 +6357,25 @@
         <v>19</v>
       </c>
       <c r="M28">
+        <v>763762000000</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="6"/>
+        <v>6499365376286.7754</v>
+      </c>
+      <c r="P28">
+        <f>K28</f>
+        <v>471773396</v>
+      </c>
+      <c r="Q28">
         <f t="shared" si="5"/>
-        <v>6499365376286.7754</v>
-      </c>
-      <c r="N28">
-        <f t="shared" si="6"/>
-        <v>471773396</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+        <v>763762000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1977</v>
       </c>
@@ -6124,15 +6413,25 @@
         <v>19</v>
       </c>
       <c r="M29">
+        <v>818300000000</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="6"/>
+        <v>7350784222229.7803</v>
+      </c>
+      <c r="P29">
+        <f>K29</f>
+        <v>513269292</v>
+      </c>
+      <c r="Q29">
         <f t="shared" si="5"/>
-        <v>7350784222229.7803</v>
-      </c>
-      <c r="N29">
-        <f t="shared" si="6"/>
-        <v>513269292</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+        <v>818300000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1978</v>
       </c>
@@ -6170,15 +6469,25 @@
         <v>19</v>
       </c>
       <c r="M30">
+        <v>936352000000</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="6"/>
+        <v>8656534451012.9414</v>
+      </c>
+      <c r="P30">
+        <f>K30</f>
+        <v>576090004</v>
+      </c>
+      <c r="Q30">
         <f t="shared" si="5"/>
-        <v>8656534451012.9414</v>
-      </c>
-      <c r="N30">
-        <f t="shared" si="6"/>
-        <v>576090004</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+        <v>936352000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1979</v>
       </c>
@@ -6216,15 +6525,25 @@
         <v>19</v>
       </c>
       <c r="M31">
+        <v>1060236000000</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="6"/>
+        <v>10054211373082.848</v>
+      </c>
+      <c r="P31">
+        <f>K31</f>
+        <v>648400600</v>
+      </c>
+      <c r="Q31">
         <f t="shared" si="5"/>
-        <v>10054211373082.848</v>
-      </c>
-      <c r="N31">
-        <f t="shared" si="6"/>
-        <v>648400600</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1060236000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1980</v>
       </c>
@@ -6262,15 +6581,25 @@
         <v>19</v>
       </c>
       <c r="M32">
+        <v>1089128000000</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="6"/>
+        <v>11336590644916.459</v>
+      </c>
+      <c r="P32">
+        <f>K32</f>
+        <v>641872888</v>
+      </c>
+      <c r="Q32">
         <f t="shared" si="5"/>
-        <v>11336590644916.459</v>
-      </c>
-      <c r="N32">
-        <f t="shared" si="6"/>
-        <v>641872888</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1089128000000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1981</v>
       </c>
@@ -6308,15 +6637,25 @@
         <v>19</v>
       </c>
       <c r="M33">
+        <v>1119066000000</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="6"/>
+        <v>11727603962156.197</v>
+      </c>
+      <c r="P33">
+        <f>K33</f>
+        <v>640619400</v>
+      </c>
+      <c r="Q33">
         <f t="shared" si="5"/>
-        <v>11727603962156.197</v>
-      </c>
-      <c r="N33">
-        <f t="shared" si="6"/>
-        <v>640619400</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1119066000000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1982</v>
       </c>
@@ -6354,15 +6693,25 @@
         <v>19</v>
       </c>
       <c r="M34">
+        <v>1142193000000</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="6"/>
+        <v>11609770331649.207</v>
+      </c>
+      <c r="P34">
+        <f>K34</f>
+        <v>654482108</v>
+      </c>
+      <c r="Q34">
         <f t="shared" si="5"/>
-        <v>11609770331649.207</v>
-      </c>
-      <c r="N34">
-        <f t="shared" si="6"/>
-        <v>654482108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1142193000000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1983</v>
       </c>
@@ -6400,15 +6749,25 @@
         <v>19</v>
       </c>
       <c r="M35">
+        <v>1189767000000</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="6"/>
+        <v>11840065192866.523</v>
+      </c>
+      <c r="P35">
+        <f>K35</f>
+        <v>685101596</v>
+      </c>
+      <c r="Q35">
         <f t="shared" si="5"/>
-        <v>11840065192866.523</v>
-      </c>
-      <c r="N35">
-        <f t="shared" si="6"/>
-        <v>685101596</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1189767000000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1984</v>
       </c>
@@ -6446,15 +6805,25 @@
         <v>19</v>
       </c>
       <c r="M36">
+        <v>1278176000000</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="6"/>
+        <v>12271599306473.012</v>
+      </c>
+      <c r="P36">
+        <f>K36</f>
+        <v>732410288</v>
+      </c>
+      <c r="Q36">
         <f t="shared" si="5"/>
-        <v>12271599306473.012</v>
-      </c>
-      <c r="N36">
-        <f t="shared" si="6"/>
-        <v>732410288</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1278176000000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1985</v>
       </c>
@@ -6492,15 +6861,25 @@
         <v>19</v>
       </c>
       <c r="M37">
+        <v>1367347000000</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="6"/>
+        <v>12862129922841.221</v>
+      </c>
+      <c r="P37">
+        <f>K37</f>
+        <v>783198104</v>
+      </c>
+      <c r="Q37">
         <f t="shared" si="5"/>
-        <v>12862129922841.221</v>
-      </c>
-      <c r="N37">
-        <f t="shared" si="6"/>
-        <v>783198104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1367347000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1986</v>
       </c>
@@ -6538,15 +6917,25 @@
         <v>19</v>
       </c>
       <c r="M38">
+        <v>1452055000000</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="6"/>
+        <v>15207735012459.988</v>
+      </c>
+      <c r="P38">
+        <f>K38</f>
+        <v>842594296</v>
+      </c>
+      <c r="Q38">
         <f t="shared" si="5"/>
-        <v>15207735012459.988</v>
-      </c>
-      <c r="N38">
-        <f t="shared" si="6"/>
-        <v>842594296</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1452055000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1987</v>
       </c>
@@ -6584,15 +6973,25 @@
         <v>19</v>
       </c>
       <c r="M39">
+        <v>1589467000000</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="6"/>
+        <v>17310212349485.184</v>
+      </c>
+      <c r="P39">
+        <f>K39</f>
+        <v>904838104</v>
+      </c>
+      <c r="Q39">
         <f t="shared" si="5"/>
-        <v>17310212349485.184</v>
-      </c>
-      <c r="N39">
-        <f t="shared" si="6"/>
-        <v>904838104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1589467000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1988</v>
       </c>
@@ -6630,15 +7029,25 @@
         <v>19</v>
       </c>
       <c r="M40">
+        <v>1705432000000</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="6"/>
+        <v>19341190141116.691</v>
+      </c>
+      <c r="P40">
+        <f>K40</f>
+        <v>953896012</v>
+      </c>
+      <c r="Q40">
         <f t="shared" si="5"/>
-        <v>19341190141116.691</v>
-      </c>
-      <c r="N40">
-        <f t="shared" si="6"/>
-        <v>953896012</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1705432000000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1989</v>
       </c>
@@ -6676,15 +7085,25 @@
         <v>19</v>
       </c>
       <c r="M41">
+        <v>1773703000000</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="6"/>
+        <v>20197416427770.797</v>
+      </c>
+      <c r="P41">
+        <f>K41</f>
+        <v>983208800</v>
+      </c>
+      <c r="Q41">
         <f t="shared" si="5"/>
-        <v>20197416427770.797</v>
-      </c>
-      <c r="N41">
-        <f t="shared" si="6"/>
-        <v>983208800</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1773703000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1990</v>
       </c>
@@ -6722,15 +7141,25 @@
         <v>19</v>
       </c>
       <c r="M42">
+        <v>1894245000000</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="6"/>
+        <v>22783754938461.852</v>
+      </c>
+      <c r="P42">
+        <f>K42</f>
+        <v>1024976616</v>
+      </c>
+      <c r="Q42">
         <f t="shared" si="5"/>
-        <v>22783754938461.852</v>
-      </c>
-      <c r="N42">
-        <f t="shared" si="6"/>
-        <v>1024976616</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1894245000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1991</v>
       </c>
@@ -6768,15 +7197,25 @@
         <v>19</v>
       </c>
       <c r="M43">
+        <v>1845418000000</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="6"/>
+        <v>23763495621881.277</v>
+      </c>
+      <c r="P43">
+        <f>K43</f>
+        <v>1133228204</v>
+      </c>
+      <c r="Q43">
         <f t="shared" si="5"/>
-        <v>23763495621881.277</v>
-      </c>
-      <c r="N43">
-        <f t="shared" si="6"/>
-        <v>1133228204</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1845418000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1992</v>
       </c>
@@ -6814,15 +7253,25 @@
         <v>19</v>
       </c>
       <c r="M44">
+        <v>1928922000000</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="6"/>
+        <v>25410281534978.652</v>
+      </c>
+      <c r="P44">
+        <f>K44</f>
+        <v>1145436692</v>
+      </c>
+      <c r="Q44">
         <f t="shared" si="5"/>
-        <v>25410281534978.652</v>
-      </c>
-      <c r="N44">
-        <f t="shared" si="6"/>
-        <v>1145436692</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1928922000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1993</v>
       </c>
@@ -6860,15 +7309,25 @@
         <v>19</v>
       </c>
       <c r="M45">
+        <v>1949421000000</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="6"/>
+        <v>25826196199251.805</v>
+      </c>
+      <c r="P45">
+        <f>K45</f>
+        <v>1142265216</v>
+      </c>
+      <c r="Q45">
         <f t="shared" si="5"/>
-        <v>25826196199251.805</v>
-      </c>
-      <c r="N45">
-        <f t="shared" si="6"/>
-        <v>1142265216</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1949421000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1994</v>
       </c>
@@ -6906,15 +7365,25 @@
         <v>19</v>
       </c>
       <c r="M46">
+        <v>2099936000000</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="6"/>
+        <v>27876766197809</v>
+      </c>
+      <c r="P46">
+        <f>K46</f>
+        <v>1233233404</v>
+      </c>
+      <c r="Q46">
         <f t="shared" si="5"/>
-        <v>27876766197809</v>
-      </c>
-      <c r="N46">
-        <f t="shared" si="6"/>
-        <v>1233233404</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+        <v>2099936000000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1995</v>
       </c>
@@ -6952,15 +7421,25 @@
         <v>19</v>
       </c>
       <c r="M47">
+        <v>2248215000000</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="6"/>
+        <v>31048402318515.469</v>
+      </c>
+      <c r="P47">
+        <f>K47</f>
+        <v>1302891640.0999999</v>
+      </c>
+      <c r="Q47">
         <f t="shared" si="5"/>
-        <v>31048402318515.469</v>
-      </c>
-      <c r="N47">
-        <f t="shared" si="6"/>
-        <v>1302891640.0999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+        <v>2248215000000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1996</v>
       </c>
@@ -6998,15 +7477,25 @@
         <v>19</v>
       </c>
       <c r="M48">
+        <v>2431695000000</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="6"/>
+        <v>31741779852478.004</v>
+      </c>
+      <c r="P48">
+        <f>K48</f>
+        <v>1390963704</v>
+      </c>
+      <c r="Q48">
         <f t="shared" si="5"/>
-        <v>31741779852478.004</v>
-      </c>
-      <c r="N48">
-        <f t="shared" si="6"/>
-        <v>1390963704</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+        <v>2431695000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1997</v>
       </c>
@@ -7044,15 +7533,25 @@
         <v>19</v>
       </c>
       <c r="M49">
+        <v>2573010000000</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="6"/>
+        <v>31627744822233.418</v>
+      </c>
+      <c r="P49">
+        <f>K49</f>
+        <v>1455104192</v>
+      </c>
+      <c r="Q49">
         <f t="shared" si="5"/>
-        <v>31627744822233.418</v>
-      </c>
-      <c r="N49">
-        <f t="shared" si="6"/>
-        <v>1455104192</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+        <v>2573010000000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1998</v>
       </c>
@@ -7090,15 +7589,25 @@
         <v>19</v>
       </c>
       <c r="M50">
+        <v>2628116000000</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="6"/>
+        <v>31546478648028.137</v>
+      </c>
+      <c r="P50">
+        <f>K50</f>
+        <v>1466961780</v>
+      </c>
+      <c r="Q50">
         <f t="shared" si="5"/>
-        <v>31546478648028.137</v>
-      </c>
-      <c r="N50">
-        <f t="shared" si="6"/>
-        <v>1466961780</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+        <v>2628116000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1999</v>
       </c>
@@ -7136,15 +7645,25 @@
         <v>19</v>
       </c>
       <c r="M51">
+        <v>2797803000000</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="6"/>
+        <v>32745401790419.211</v>
+      </c>
+      <c r="P51">
+        <f>K51</f>
+        <v>1562256300</v>
+      </c>
+      <c r="Q51">
         <f t="shared" si="5"/>
-        <v>32745401790419.211</v>
-      </c>
-      <c r="N51">
-        <f t="shared" si="6"/>
-        <v>1562256300</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+        <v>2797803000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2000</v>
       </c>
@@ -7182,15 +7701,25 @@
         <v>19</v>
       </c>
       <c r="M52">
+        <v>3201366124113.3198</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="6"/>
+        <v>33839543447259.059</v>
+      </c>
+      <c r="P52">
+        <f>K52</f>
+        <v>1674064712</v>
+      </c>
+      <c r="Q52">
         <f t="shared" si="5"/>
-        <v>33839543447259.059</v>
-      </c>
-      <c r="N52">
-        <f t="shared" si="6"/>
-        <v>1674064712</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3201366124113.3198</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2001</v>
       </c>
@@ -7228,15 +7757,25 @@
         <v>19</v>
       </c>
       <c r="M53">
+        <v>3108526506514.0298</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="6"/>
+        <v>33623874142346.625</v>
+      </c>
+      <c r="P53">
+        <f>K53</f>
+        <v>1655230214</v>
+      </c>
+      <c r="Q53">
         <f t="shared" si="5"/>
-        <v>33623874142346.625</v>
-      </c>
-      <c r="N53">
-        <f t="shared" si="6"/>
-        <v>1655230214</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3108526506514.0298</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2002</v>
       </c>
@@ -7274,15 +7813,25 @@
         <v>19</v>
       </c>
       <c r="M54">
+        <v>3124069139046.6001</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="6"/>
+        <v>34917872758829.059</v>
+      </c>
+      <c r="P54">
+        <f>K54</f>
+        <v>1627404873</v>
+      </c>
+      <c r="Q54">
         <f t="shared" si="5"/>
-        <v>34917872758829.059</v>
-      </c>
-      <c r="N54">
-        <f t="shared" si="6"/>
-        <v>1627404873</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3124069139046.6001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2003</v>
       </c>
@@ -7320,15 +7869,25 @@
         <v>19</v>
       </c>
       <c r="M55">
+        <v>3180302383549.4399</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="6"/>
+        <v>39152219944703.523</v>
+      </c>
+      <c r="P55">
+        <f>K55</f>
+        <v>1665309283</v>
+      </c>
+      <c r="Q55">
         <f t="shared" si="5"/>
-        <v>39152219944703.523</v>
-      </c>
-      <c r="N55">
-        <f t="shared" si="6"/>
-        <v>1665309283</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3180302383549.4399</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2004</v>
       </c>
@@ -7366,15 +7925,25 @@
         <v>19</v>
       </c>
       <c r="M56">
+        <v>3628725019629.9102</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="6"/>
+        <v>44123871631674.5</v>
+      </c>
+      <c r="P56">
+        <f>K56</f>
+        <v>1888695284</v>
+      </c>
+      <c r="Q56">
         <f t="shared" si="5"/>
-        <v>44123871631674.5</v>
-      </c>
-      <c r="N56">
-        <f t="shared" si="6"/>
-        <v>1888695284</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3628725019629.9102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2005</v>
       </c>
@@ -7412,15 +7981,25 @@
         <v>19</v>
       </c>
       <c r="M57">
+        <v>3919023021200.2998</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="6"/>
+        <v>47784318320003.891</v>
+      </c>
+      <c r="P57">
+        <f>K57</f>
+        <v>1969590799</v>
+      </c>
+      <c r="Q57">
         <f t="shared" si="5"/>
-        <v>47784318320003.891</v>
-      </c>
-      <c r="N57">
-        <f t="shared" si="6"/>
-        <v>1969590799</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3919023021200.2998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2006</v>
       </c>
@@ -7458,15 +8037,25 @@
         <v>19</v>
       </c>
       <c r="M58">
+        <v>4170556195914.7002</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="6"/>
+        <v>51780102663354.961</v>
+      </c>
+      <c r="P58">
+        <f>K58</f>
+        <v>2072413898</v>
+      </c>
+      <c r="Q58">
         <f t="shared" si="5"/>
-        <v>51780102663354.961</v>
-      </c>
-      <c r="N58">
-        <f t="shared" si="6"/>
-        <v>2072413898</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+        <v>4170556195914.7002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2007</v>
       </c>
@@ -7504,15 +8093,25 @@
         <v>19</v>
       </c>
       <c r="M59">
+        <v>4513095886534.6602</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="6"/>
+        <v>58349348476252.422</v>
+      </c>
+      <c r="P59">
+        <f>K59</f>
+        <v>2209136496</v>
+      </c>
+      <c r="Q59">
         <f t="shared" si="5"/>
-        <v>58349348476252.422</v>
-      </c>
-      <c r="N59">
-        <f t="shared" si="6"/>
-        <v>2209136496</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+        <v>4513095886534.6602</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2008</v>
       </c>
@@ -7550,15 +8149,25 @@
         <v>19</v>
       </c>
       <c r="M60">
+        <v>4608466258169.2598</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="6"/>
+        <v>64120604168598.344</v>
+      </c>
+      <c r="P60">
+        <f>K60</f>
+        <v>2208218737</v>
+      </c>
+      <c r="Q60">
         <f t="shared" si="5"/>
-        <v>64120604168598.344</v>
-      </c>
-      <c r="N60">
-        <f t="shared" si="6"/>
-        <v>2208218737</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+        <v>4608466258169.2598</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2009</v>
       </c>
@@ -7596,15 +8205,25 @@
         <v>19</v>
       </c>
       <c r="M61">
+        <v>4561413042719.0596</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="6"/>
+        <v>60803913019546.531</v>
+      </c>
+      <c r="P61">
+        <f>K61</f>
+        <v>2249728546</v>
+      </c>
+      <c r="Q61">
         <f t="shared" si="5"/>
-        <v>60803913019546.531</v>
-      </c>
-      <c r="N61">
-        <f t="shared" si="6"/>
-        <v>2249728546</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+        <v>4561413042719.0596</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2010</v>
       </c>
@@ -7642,15 +8261,25 @@
         <v>19</v>
       </c>
       <c r="M62">
+        <v>4930250015715.4404</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="6"/>
+        <v>66605599347148.477</v>
+      </c>
+      <c r="P62">
+        <f>K62</f>
+        <v>2669414339.2099419</v>
+      </c>
+      <c r="Q62">
         <f t="shared" si="5"/>
-        <v>66605599347148.477</v>
-      </c>
-      <c r="N62">
-        <f t="shared" si="6"/>
-        <v>2669414339.2099419</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+        <v>4930250015715.4404</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2011</v>
       </c>
@@ -7688,15 +8317,25 @@
         <v>19</v>
       </c>
       <c r="M63">
+        <v>5263525000000</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="6"/>
+        <v>73857461479872.312</v>
+      </c>
+      <c r="P63">
+        <f>K63</f>
+        <v>2833214050.1820679</v>
+      </c>
+      <c r="Q63">
         <f t="shared" si="5"/>
-        <v>73857461479872.312</v>
-      </c>
-      <c r="N63">
-        <f t="shared" si="6"/>
-        <v>2833214050.1820679</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+        <v>5263525000000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2012</v>
       </c>
@@ -7734,15 +8373,25 @@
         <v>19</v>
       </c>
       <c r="M64">
+        <v>5537024000000</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="6"/>
+        <v>75500388177983.547</v>
+      </c>
+      <c r="P64">
+        <f>K64</f>
+        <v>2943247912.564888</v>
+      </c>
+      <c r="Q64">
         <f t="shared" si="5"/>
-        <v>75500388177983.547</v>
-      </c>
-      <c r="N64">
-        <f t="shared" si="6"/>
-        <v>2943247912.564888</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+        <v>5537024000000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2013</v>
       </c>
@@ -7780,15 +8429,25 @@
         <v>19</v>
       </c>
       <c r="M65">
+        <v>5841156000000</v>
+      </c>
+      <c r="N65" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="6"/>
+        <v>77606228872413.938</v>
+      </c>
+      <c r="P65">
+        <f>K65</f>
+        <v>3100200780.1726723</v>
+      </c>
+      <c r="Q65">
         <f t="shared" si="5"/>
-        <v>77606228872413.938</v>
-      </c>
-      <c r="N65">
-        <f t="shared" si="6"/>
-        <v>3100200780.1726723</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+        <v>5841156000000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2014</v>
       </c>
@@ -7826,15 +8485,25 @@
         <v>19</v>
       </c>
       <c r="M66">
+        <v>6190282000000</v>
+      </c>
+      <c r="N66" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="6"/>
+        <v>79732636600985.5</v>
+      </c>
+      <c r="P66">
+        <f>K66</f>
+        <v>3285080769.4758945</v>
+      </c>
+      <c r="Q66">
         <f t="shared" si="5"/>
-        <v>79732636600985.5</v>
-      </c>
-      <c r="N66">
-        <f t="shared" si="6"/>
-        <v>3285080769.4758945</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+        <v>6190282000000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2015</v>
       </c>
@@ -7872,15 +8541,25 @@
         <v>19</v>
       </c>
       <c r="M67">
-        <f t="shared" si="5"/>
+        <v>6654454000000</v>
+      </c>
+      <c r="N67" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="6"/>
         <v>75186364779691.656</v>
       </c>
-      <c r="N67">
-        <f t="shared" si="6"/>
+      <c r="P67">
+        <f>K67</f>
         <v>3525115153</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q67">
+        <f t="shared" ref="Q67:Q74" si="7">M67</f>
+        <v>6654454000000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2016</v>
       </c>
@@ -7918,15 +8597,25 @@
         <v>19</v>
       </c>
       <c r="M68">
-        <f t="shared" si="5"/>
+        <v>7146283000000</v>
+      </c>
+      <c r="N68" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="6"/>
         <v>76469364472137.875</v>
       </c>
-      <c r="N68">
-        <f t="shared" si="6"/>
+      <c r="P68">
+        <f>K68</f>
         <v>3760774350</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q68">
+        <f t="shared" si="7"/>
+        <v>7146283000000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2017</v>
       </c>
@@ -7964,15 +8653,25 @@
         <v>19</v>
       </c>
       <c r="M69">
-        <f t="shared" si="5"/>
+        <v>7718470000000</v>
+      </c>
+      <c r="N69" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="6"/>
         <v>81409498368206.078</v>
       </c>
-      <c r="N69">
-        <f t="shared" si="6"/>
+      <c r="P69">
+        <f>K69</f>
         <v>4025616011.7703109</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q69">
+        <f t="shared" si="7"/>
+        <v>7718470000000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2018</v>
       </c>
@@ -8010,15 +8709,25 @@
         <v>19</v>
       </c>
       <c r="M70">
-        <f t="shared" si="5"/>
+        <v>8280851000000</v>
+      </c>
+      <c r="N70" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O70">
+        <f t="shared" si="6"/>
         <v>86466958777951.672</v>
       </c>
-      <c r="N70">
-        <f t="shared" si="6"/>
+      <c r="P70">
+        <f>K70</f>
         <v>4293921426.1293054</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q70">
+        <f t="shared" si="7"/>
+        <v>8280851000000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2019</v>
       </c>
@@ -8056,15 +8765,25 @@
         <v>19</v>
       </c>
       <c r="M71">
-        <f t="shared" si="5"/>
+        <v>8664032000000</v>
+      </c>
+      <c r="N71" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O71">
+        <f t="shared" si="6"/>
         <v>87654250895445.703</v>
       </c>
-      <c r="N71">
-        <f t="shared" si="6"/>
+      <c r="P71">
+        <f>K71</f>
         <v>4455690101.0282774</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q71">
+        <f t="shared" si="7"/>
+        <v>8664032000000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2020</v>
       </c>
@@ -8102,15 +8821,25 @@
         <v>19</v>
       </c>
       <c r="M72">
-        <f t="shared" si="5"/>
+        <v>2962287000000</v>
+      </c>
+      <c r="N72" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O72">
+        <f t="shared" si="6"/>
         <v>85116336691718.734</v>
       </c>
-      <c r="N72">
-        <f t="shared" si="6"/>
+      <c r="P72">
+        <f>K72</f>
         <v>1771894087.0245001</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q72">
+        <f t="shared" si="7"/>
+        <v>2962287000000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2021</v>
       </c>
@@ -8148,15 +8877,25 @@
         <v>19</v>
       </c>
       <c r="M73">
-        <f t="shared" si="5"/>
+        <v>3626024000000</v>
+      </c>
+      <c r="N73" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O73">
+        <f t="shared" si="6"/>
         <v>96527425918257.781</v>
       </c>
-      <c r="N73">
-        <f t="shared" si="6"/>
+      <c r="P73">
+        <f>K73</f>
         <v>2279974770.1229997</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q73">
+        <f t="shared" si="7"/>
+        <v>3626024000000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2022</v>
       </c>
@@ -8187,8 +8926,16 @@
       <c r="L74" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M74">
-        <f t="shared" si="5"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O74">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q74">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -8321,6 +9068,79 @@
     <hyperlink ref="L69" r:id="rId125" xr:uid="{A9A4A693-75F5-9849-A7AE-6DA4A3EC57AE}"/>
     <hyperlink ref="L71" r:id="rId126" xr:uid="{B1E7DEC6-66C1-6243-AC11-B589A26DABE4}"/>
     <hyperlink ref="L73" r:id="rId127" xr:uid="{5BB5D593-63FA-5041-938A-8DD8007119C5}"/>
+    <hyperlink ref="N2" r:id="rId128" xr:uid="{A1D0B79F-E0F3-5749-B590-CB73FE3D2FCB}"/>
+    <hyperlink ref="N3" r:id="rId129" xr:uid="{48A8B0E0-A393-D54D-984E-AD3C4A153F13}"/>
+    <hyperlink ref="N4" r:id="rId130" xr:uid="{F3CC9FBE-C155-8D4E-B150-EA324A2A1AD3}"/>
+    <hyperlink ref="N6" r:id="rId131" xr:uid="{EE01C391-07C6-1D47-95F3-B5D6D108658B}"/>
+    <hyperlink ref="N8" r:id="rId132" xr:uid="{0AC6B22B-2258-4B43-8608-C000160D5691}"/>
+    <hyperlink ref="N10" r:id="rId133" xr:uid="{552514F9-D17E-6648-83A5-4D5563744BA4}"/>
+    <hyperlink ref="N12" r:id="rId134" xr:uid="{0A2F9344-2557-064B-91A6-2700D4D88620}"/>
+    <hyperlink ref="N14" r:id="rId135" xr:uid="{4D9C13C8-A711-7C43-B214-59E59B50D7D7}"/>
+    <hyperlink ref="N16" r:id="rId136" xr:uid="{75F28EF9-4BD7-7349-98F6-577DFF2CF0A3}"/>
+    <hyperlink ref="N18" r:id="rId137" xr:uid="{2C1ED721-C639-FB4F-B201-ADB51E727492}"/>
+    <hyperlink ref="N20" r:id="rId138" xr:uid="{21B2117F-1C53-6848-A24F-905EA6FB1E77}"/>
+    <hyperlink ref="N22" r:id="rId139" xr:uid="{09FAB061-D2E8-F346-8B43-231110219690}"/>
+    <hyperlink ref="N24" r:id="rId140" xr:uid="{9F81D91D-DCE5-D749-BA99-F262968BC5E3}"/>
+    <hyperlink ref="N26" r:id="rId141" xr:uid="{4BEF474F-39AE-2E4E-8355-78FBCF0E4C48}"/>
+    <hyperlink ref="N28" r:id="rId142" xr:uid="{72B16E52-3A74-6844-92D3-C69F1AF9DC11}"/>
+    <hyperlink ref="N30" r:id="rId143" xr:uid="{E8674593-5F6B-E84A-ADB7-BB05786FA3BD}"/>
+    <hyperlink ref="N32" r:id="rId144" xr:uid="{A45739D0-2F08-C945-A611-3194AE1AAC59}"/>
+    <hyperlink ref="N34" r:id="rId145" xr:uid="{50E09D92-3916-E54F-A6A8-4A0EDCAC66CD}"/>
+    <hyperlink ref="N36" r:id="rId146" xr:uid="{C086F778-F914-B643-B9BB-19FCD4015837}"/>
+    <hyperlink ref="N38" r:id="rId147" xr:uid="{D79FBFE7-1198-3F41-A006-3AFCC2FC2E92}"/>
+    <hyperlink ref="N40" r:id="rId148" xr:uid="{56143922-12D2-8847-9874-A8379CDBC70A}"/>
+    <hyperlink ref="N42" r:id="rId149" xr:uid="{F7AA5E29-F4F7-EE49-A2B5-C560D46E211D}"/>
+    <hyperlink ref="N44" r:id="rId150" xr:uid="{CBC69C1B-678E-C74B-9540-1F6AA6A6B5B3}"/>
+    <hyperlink ref="N46" r:id="rId151" xr:uid="{9AD80CED-3402-F041-BC82-534304BFF37A}"/>
+    <hyperlink ref="N48" r:id="rId152" xr:uid="{EF84B52E-B12F-A047-BBC1-E1B4E5C8B6FD}"/>
+    <hyperlink ref="N50" r:id="rId153" xr:uid="{25542899-6C47-E243-9A7B-BA9F3054B2D8}"/>
+    <hyperlink ref="N52" r:id="rId154" xr:uid="{C541AB8F-1B57-3E40-B3F1-FDA389BA7D3D}"/>
+    <hyperlink ref="N54" r:id="rId155" xr:uid="{43339395-39CC-A34C-9BE3-07673C8B28CC}"/>
+    <hyperlink ref="N56" r:id="rId156" xr:uid="{87F5C69F-8A68-854F-AAA0-A748B6567520}"/>
+    <hyperlink ref="N58" r:id="rId157" xr:uid="{5939673F-F2CE-F540-AA28-E0FB71D7E7C8}"/>
+    <hyperlink ref="N60" r:id="rId158" xr:uid="{FEF0E02F-7E03-5849-9B6E-0D3F916C10DD}"/>
+    <hyperlink ref="N62" r:id="rId159" xr:uid="{0D692AD2-532E-C54D-B8A7-8FF9B9226145}"/>
+    <hyperlink ref="N64" r:id="rId160" xr:uid="{54F85B45-11CD-E94D-A50A-3223229CDD50}"/>
+    <hyperlink ref="N66" r:id="rId161" xr:uid="{A2E10D00-0C5B-934B-ABF7-9A72C80F10B2}"/>
+    <hyperlink ref="N68" r:id="rId162" xr:uid="{D4FD1509-4346-0E4F-9AC4-665FB160313F}"/>
+    <hyperlink ref="N70" r:id="rId163" xr:uid="{C53C2D1C-4F7B-6C49-A3E5-64D5FABC0E50}"/>
+    <hyperlink ref="N72" r:id="rId164" xr:uid="{5A232810-10E4-0D46-BCB7-A98196583EBE}"/>
+    <hyperlink ref="N74" r:id="rId165" xr:uid="{E63DC2C0-A307-F645-A8BB-39D60EEF08BF}"/>
+    <hyperlink ref="N5" r:id="rId166" xr:uid="{D81A40FC-86FE-CF45-B6C2-65296E87E30E}"/>
+    <hyperlink ref="N7" r:id="rId167" xr:uid="{5DFC8CB9-0D56-3D48-9B08-F397CA025665}"/>
+    <hyperlink ref="N9" r:id="rId168" xr:uid="{20A87250-E53E-5448-A4D6-9F4CFBAC199B}"/>
+    <hyperlink ref="N11" r:id="rId169" xr:uid="{0048B03F-BF96-054A-B6AC-B6B0CF09A8E0}"/>
+    <hyperlink ref="N13" r:id="rId170" xr:uid="{DE61AF7D-0BF4-2D4E-AE5A-D94E74B4F193}"/>
+    <hyperlink ref="N15" r:id="rId171" xr:uid="{188AE8E1-D8AC-2D43-928B-9CAE6E7C9422}"/>
+    <hyperlink ref="N17" r:id="rId172" xr:uid="{61ABCBB2-299D-1843-9A62-7692179BD50A}"/>
+    <hyperlink ref="N19" r:id="rId173" xr:uid="{BAF503F9-8CC9-8D41-A7D1-182E02044A74}"/>
+    <hyperlink ref="N21" r:id="rId174" xr:uid="{8FCBE077-EB18-1042-85BB-A0CAF333B835}"/>
+    <hyperlink ref="N23" r:id="rId175" xr:uid="{4A8CD7F8-B5F5-9745-9038-A4107742C85F}"/>
+    <hyperlink ref="N25" r:id="rId176" xr:uid="{88306C83-94D4-3C4B-9F35-56C6A154AF8B}"/>
+    <hyperlink ref="N27" r:id="rId177" xr:uid="{A56AD099-CFAB-6046-80DB-A782D5FADC7B}"/>
+    <hyperlink ref="N29" r:id="rId178" xr:uid="{2F49746B-268C-EE4A-B862-91777BC42D62}"/>
+    <hyperlink ref="N31" r:id="rId179" xr:uid="{EE0AE332-8136-064E-83EB-E3864CD07D58}"/>
+    <hyperlink ref="N33" r:id="rId180" xr:uid="{796957AB-19C9-C845-841A-0BA8663F11FA}"/>
+    <hyperlink ref="N35" r:id="rId181" xr:uid="{943A5407-A154-EE4A-ABBB-EB2D393EC813}"/>
+    <hyperlink ref="N37" r:id="rId182" xr:uid="{BD491053-D72D-7042-B48E-CE54BB8631D2}"/>
+    <hyperlink ref="N39" r:id="rId183" xr:uid="{834EE6DA-9FDF-4342-9B03-0770760D4D71}"/>
+    <hyperlink ref="N41" r:id="rId184" xr:uid="{79D6366A-2A29-4C4B-8A86-09CA5277A7DD}"/>
+    <hyperlink ref="N43" r:id="rId185" xr:uid="{F5B1D6EF-5C99-6545-827F-09A33481CA16}"/>
+    <hyperlink ref="N45" r:id="rId186" xr:uid="{BBE81267-9C9B-8241-A136-8C2684AFFA6E}"/>
+    <hyperlink ref="N47" r:id="rId187" xr:uid="{15045998-2DA6-524E-B9E5-8BE191296449}"/>
+    <hyperlink ref="N49" r:id="rId188" xr:uid="{20F2DE59-DE98-384C-822F-9FDE6F9F563C}"/>
+    <hyperlink ref="N51" r:id="rId189" xr:uid="{2860BBE4-0ABE-834B-BE14-6BB5018E7B1D}"/>
+    <hyperlink ref="N53" r:id="rId190" xr:uid="{51946FC2-51B3-E94D-ADDA-1E3BE25D0D79}"/>
+    <hyperlink ref="N55" r:id="rId191" xr:uid="{66B3F614-5015-4046-814C-FDDFF90D81DC}"/>
+    <hyperlink ref="N57" r:id="rId192" xr:uid="{1CD0EF4E-D3C2-CA4A-9169-A83CFA820F84}"/>
+    <hyperlink ref="N59" r:id="rId193" xr:uid="{AE52175D-40A6-BF48-9C2A-625763CDE507}"/>
+    <hyperlink ref="N61" r:id="rId194" xr:uid="{E395533E-C8E0-1045-B711-635B94FA00A8}"/>
+    <hyperlink ref="N63" r:id="rId195" xr:uid="{DF969924-A001-EA4C-A061-CE71DA5D0854}"/>
+    <hyperlink ref="N65" r:id="rId196" xr:uid="{B107384C-7D01-8342-BA81-1DA05A17D862}"/>
+    <hyperlink ref="N67" r:id="rId197" xr:uid="{9B1F7BD8-B689-1D45-BC4D-F63A056C9770}"/>
+    <hyperlink ref="N69" r:id="rId198" xr:uid="{3C7F2AD5-8A28-1748-8416-731F1A7FC8E5}"/>
+    <hyperlink ref="N71" r:id="rId199" xr:uid="{93DE2956-051D-9B46-A498-8D28EADAF674}"/>
+    <hyperlink ref="N73" r:id="rId200" xr:uid="{2001EBDE-3349-7943-96DB-EA8B29E172C1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>